<commit_message>
updates the way assets are handled and generates sample assets
</commit_message>
<xml_diff>
--- a/basic_gui/NotionalETEOutput000.xlsx
+++ b/basic_gui/NotionalETEOutput000.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\white\Documents\etesim_gui_test\basic_gui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwhite\OneDrive - Torch Technologies, Inc\etesim_gui_test\basic_gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D959B8A-0EDB-498D-9C9F-03A5902B37A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{7D959B8A-0EDB-498D-9C9F-03A5902B37A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C190A13-3CE8-41B4-B511-23603634477A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{63FFE2E9-3229-4312-AC35-4985EA2DE2C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63FFE2E9-3229-4312-AC35-4985EA2DE2C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -96,18 +94,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,18 +433,18 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -488,7 +479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>54</v>
       </c>
@@ -504,32 +495,26 @@
       <c r="E2">
         <v>152.142</v>
       </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F8" si="0">F3</f>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G7" si="1">G3</f>
-        <v>-100</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H8" si="2">H3</f>
-        <v>858.87986642373744</v>
+      <c r="F2">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G2">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H2">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I2">
-        <f>2749.9952841403*EXP((345.846-J2)/2000) - 2702.64367585252</f>
-        <v>-1499.9999999999973</v>
+        <v>1114861.26866097</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J33" si="3">2000-48.6515882352941*(E2-152.142)</f>
-        <v>2000</v>
+        <v>4843223.2746094698</v>
       </c>
       <c r="K2">
-        <f>3200 * ( 1 - (J2-1000)*(J2-1000)/1000000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984368.3041540701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>54</v>
       </c>
@@ -545,32 +530,26 @@
       <c r="E3">
         <v>153.142</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G3" s="1">
-        <f t="shared" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F3">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G3">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H3">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I54" si="4">2749.9952841403*EXP((345.846-J3)/2000) - 2702.64367585252</f>
-        <v>-1470.3860058940224</v>
+        <v>1114890.882655076</v>
       </c>
       <c r="J3">
-        <f t="shared" si="3"/>
-        <v>1951.3484117647058</v>
+        <v>4843174.6230212348</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K54" si="5">3200 * ( 1 - (J3-1000)*(J3-1000)/1000000)</f>
-        <v>303.79583818486964</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984672.0999922547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>54</v>
       </c>
@@ -586,32 +565,26 @@
       <c r="E4">
         <v>154.142</v>
       </c>
-      <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F4">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G4">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H4">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I4">
-        <f t="shared" si="4"/>
-        <v>-1440.0427944275632</v>
+        <v>1114921.2258665424</v>
       </c>
       <c r="J4">
-        <f t="shared" si="3"/>
-        <v>1902.6968235294119</v>
+        <v>4843125.9714329988</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
-        <v>592.44302332771178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984960.7471773978</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>54</v>
       </c>
@@ -627,32 +600,26 @@
       <c r="E5">
         <v>155.142</v>
       </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F5">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G5">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H5">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I5">
-        <f t="shared" si="4"/>
-        <v>-1408.9524092939848</v>
+        <v>1114952.3162516761</v>
       </c>
       <c r="J5">
-        <f t="shared" si="3"/>
-        <v>1854.0452352941177</v>
+        <v>4843077.3198447637</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
-        <v>865.94155542852855</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985234.2457094984</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>54</v>
       </c>
@@ -668,32 +635,26 @@
       <c r="E6">
         <v>156.142</v>
       </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F6">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G6">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H6">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I6">
-        <f t="shared" si="4"/>
-        <v>-1377.0964520291222</v>
+        <v>1114984.1722089408</v>
       </c>
       <c r="J6">
-        <f t="shared" si="3"/>
-        <v>1805.3936470588237</v>
+        <v>4843028.6682565287</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
-        <v>1124.2914344873182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985492.5955885574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>54</v>
       </c>
@@ -709,32 +670,26 @@
       <c r="E7">
         <v>157.142</v>
       </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F7">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G7">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H7">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I7">
-        <f t="shared" si="4"/>
-        <v>-1344.4560711235551</v>
+        <v>1115016.8125898466</v>
       </c>
       <c r="J7">
-        <f t="shared" si="3"/>
-        <v>1756.7420588235295</v>
+        <v>4842980.0166682936</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
-        <v>1367.4926605040828</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985735.7968145744</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>54</v>
       </c>
@@ -750,32 +705,26 @@
       <c r="E8">
         <v>158.142</v>
       </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>217.43722336844749</v>
-      </c>
-      <c r="G8" s="1">
-        <f>G9</f>
-        <v>-100</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="2"/>
-        <v>858.87986642373744</v>
+      <c r="F8">
+        <v>1116578.7058843386</v>
+      </c>
+      <c r="G8">
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H8">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I8">
-        <f t="shared" si="4"/>
-        <v>-1311.0119508667885</v>
+        <v>1115050.2567101032</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
-        <v>1708.0904705882353</v>
+        <v>4842931.3650800576</v>
       </c>
       <c r="K8">
-        <f t="shared" si="5"/>
-        <v>1595.5452334788206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985963.8493875489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>54</v>
       </c>
@@ -791,32 +740,26 @@
       <c r="E9">
         <v>159.142</v>
       </c>
-      <c r="F9" s="1">
-        <f>F10</f>
-        <v>217.43722336844749</v>
+      <c r="F9">
+        <v>1116578.7058843386</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G7:G54" si="6">16.5128148148148*(E9-159.142)-100</f>
-        <v>-100</v>
-      </c>
-      <c r="H9" s="1">
-        <f>H10</f>
-        <v>858.87986642373744</v>
+        <v>4841123.2746094698</v>
+      </c>
+      <c r="H9">
+        <v>3985227.1840204936</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
-        <v>-1276.7442999167256</v>
+        <v>1115084.5243610532</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
-        <v>1659.4388823529412</v>
+        <v>4842882.7134918226</v>
       </c>
       <c r="K9">
-        <f t="shared" si="5"/>
-        <v>1808.4491534115323</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986176.7533074818</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>54</v>
       </c>
@@ -833,31 +776,25 @@
         <v>160.142</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:F54" si="7">IF(G10=-100, 0, 10*POWER(G10+100, 1.5)*POWER(SIN(10/(G10+100)),2))</f>
-        <v>217.43722336844749</v>
+        <v>1116578.7058843386</v>
       </c>
       <c r="G10">
-        <f t="shared" si="6"/>
-        <v>-83.487185185185197</v>
+        <v>4841139.787424285</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H54" si="8">300*LOG(G10+101, EXP(1))</f>
-        <v>858.87986642373744</v>
+        <v>3985227.1840204936</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
-        <v>-1241.6328395876783</v>
+        <v>1115119.6358213823</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
-        <v>1610.7872941176472</v>
+        <v>4842834.0619035875</v>
       </c>
       <c r="K10">
-        <f t="shared" si="5"/>
-        <v>2006.2044203022169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986374.5085743722</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>54</v>
       </c>
@@ -874,31 +811,25 @@
         <v>161.142</v>
       </c>
       <c r="F11">
-        <f t="shared" si="7"/>
-        <v>168.7566507903731</v>
+        <v>1116530.0253117604</v>
       </c>
       <c r="G11">
-        <f t="shared" si="6"/>
-        <v>-66.974370370370394</v>
+        <v>4841156.3002390992</v>
       </c>
       <c r="H11">
-        <f t="shared" si="8"/>
-        <v>1058.1342159834842</v>
+        <v>3985426.4383700537</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
-        <v>-1205.6567918499791</v>
+        <v>1115155.61186912</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
-        <v>1562.1357058823532</v>
+        <v>4842785.4103153525</v>
       </c>
       <c r="K11">
-        <f t="shared" si="5"/>
-        <v>2188.811034150875</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986557.115188221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>54</v>
       </c>
@@ -915,31 +846,25 @@
         <v>162.142</v>
       </c>
       <c r="F12">
-        <f t="shared" si="7"/>
-        <v>140.15925648189312</v>
+        <v>1116501.4279174518</v>
       </c>
       <c r="G12">
-        <f t="shared" si="6"/>
-        <v>-50.461555555555606</v>
+        <v>4841172.8130539143</v>
       </c>
       <c r="H12">
-        <f t="shared" si="8"/>
-        <v>1176.8202968355704</v>
+        <v>3985545.1244509057</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
-        <v>-1168.7948670340963</v>
+        <v>1115192.473793936</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
-        <v>1513.4841176470591</v>
+        <v>4842736.7587271165</v>
       </c>
       <c r="K12">
-        <f t="shared" si="5"/>
-        <v>2356.2689949575079</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986724.5731490278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>54</v>
       </c>
@@ -956,31 +881,25 @@
         <v>163.142</v>
       </c>
       <c r="F13">
-        <f t="shared" si="7"/>
-        <v>122.10648318338475</v>
+        <v>1116483.3751441534</v>
       </c>
       <c r="G13">
-        <f t="shared" si="6"/>
-        <v>-33.948740740740803</v>
+        <v>4841189.3258687295</v>
       </c>
       <c r="H13">
-        <f t="shared" si="8"/>
-        <v>1261.6372171350147</v>
+        <v>3985629.9413712053</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
-        <v>-1131.0252512319707</v>
+        <v>1115230.2434097382</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
-        <v>1464.8325294117649</v>
+        <v>4842688.1071388815</v>
       </c>
       <c r="K13">
-        <f t="shared" si="5"/>
-        <v>2508.5783027221146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986876.8824567921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>54</v>
       </c>
@@ -997,31 +916,25 @@
         <v>164.142</v>
       </c>
       <c r="F14">
-        <f t="shared" si="7"/>
-        <v>109.51655236551397</v>
+        <v>1116470.7852133357</v>
       </c>
       <c r="G14">
-        <f t="shared" si="6"/>
-        <v>-17.435925925926</v>
+        <v>4841205.8386835437</v>
       </c>
       <c r="H14">
-        <f t="shared" si="8"/>
-        <v>1327.6841075314937</v>
+        <v>3985695.9882616014</v>
       </c>
       <c r="I14">
-        <f t="shared" si="4"/>
-        <v>-1092.3255933881278</v>
+        <v>1115268.9430675819</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
-        <v>1416.1809411764707</v>
+        <v>4842639.4555506464</v>
       </c>
       <c r="K14">
-        <f t="shared" si="5"/>
-        <v>2645.7389574446947</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987014.0431115148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>54</v>
       </c>
@@ -1038,31 +951,25 @@
         <v>165.142</v>
       </c>
       <c r="F15">
-        <f t="shared" si="7"/>
-        <v>100.12408694997187</v>
+        <v>1116461.39274792</v>
       </c>
       <c r="G15">
-        <f t="shared" si="6"/>
-        <v>-0.92311111111121136</v>
+        <v>4841222.3514983589</v>
       </c>
       <c r="H15">
-        <f t="shared" si="8"/>
-        <v>1381.7816338300049</v>
+        <v>3985750.0857879003</v>
       </c>
       <c r="I15">
-        <f t="shared" si="4"/>
-        <v>-1052.6729920729126</v>
+        <v>1115308.595668897</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
-        <v>1367.5293529411767</v>
+        <v>4842590.8039624114</v>
       </c>
       <c r="K15">
-        <f t="shared" si="5"/>
-        <v>2767.7509591252478</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987136.0551131954</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>54</v>
       </c>
@@ -1079,31 +986,25 @@
         <v>166.142</v>
       </c>
       <c r="F16">
-        <f t="shared" si="7"/>
-        <v>92.78049061392791</v>
+        <v>1116454.049151584</v>
       </c>
       <c r="G16">
-        <f t="shared" si="6"/>
-        <v>15.589703703703591</v>
+        <v>4841238.8643131731</v>
       </c>
       <c r="H16">
-        <f t="shared" si="8"/>
-        <v>1427.5982896768196</v>
+        <v>3985795.902443747</v>
       </c>
       <c r="I16">
-        <f t="shared" si="4"/>
-        <v>-1012.0439819300345</v>
+        <v>1115349.22467904</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
-        <v>1318.8777647058826</v>
+        <v>4842542.1523741754</v>
       </c>
       <c r="K16">
-        <f t="shared" si="5"/>
-        <v>2874.6143077637753</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987242.9184618341</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>54</v>
       </c>
@@ -1120,31 +1021,25 @@
         <v>167.142</v>
       </c>
       <c r="F17">
-        <f t="shared" si="7"/>
-        <v>86.838986473286141</v>
+        <v>1116448.1076474434</v>
       </c>
       <c r="G17">
-        <f t="shared" si="6"/>
-        <v>32.102518518518394</v>
+        <v>4841255.3771279883</v>
       </c>
       <c r="H17">
-        <f t="shared" si="8"/>
-        <v>1467.3358941673318</v>
+        <v>3985835.6400482375</v>
       </c>
       <c r="I17">
-        <f t="shared" si="4"/>
-        <v>-970.41451979039175</v>
+        <v>1115390.8541411797</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
-        <v>1270.2261764705886</v>
+        <v>4842493.5007859403</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
-        <v>2966.3290033602761</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987334.6331574302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>54</v>
       </c>
@@ -1161,31 +1056,25 @@
         <v>168.142</v>
       </c>
       <c r="F18">
-        <f t="shared" si="7"/>
-        <v>81.905420960027143</v>
+        <v>1116443.17408193</v>
       </c>
       <c r="G18">
-        <f t="shared" si="6"/>
-        <v>48.615333333333183</v>
+        <v>4841271.8899428034</v>
       </c>
       <c r="H18">
-        <f t="shared" si="8"/>
-        <v>1502.4202667495215</v>
+        <v>3985870.7244208194</v>
       </c>
       <c r="I18">
-        <f t="shared" si="4"/>
-        <v>-927.75997044396354</v>
+        <v>1115433.508690526</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
-        <v>1221.5745882352944</v>
+        <v>4842444.8491977053</v>
       </c>
       <c r="K18">
-        <f t="shared" si="5"/>
-        <v>3042.8950459147513</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987411.1991999848</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>54</v>
       </c>
@@ -1202,31 +1091,25 @@
         <v>169.142</v>
       </c>
       <c r="F19">
-        <f t="shared" si="7"/>
-        <v>77.724595392222582</v>
+        <v>1116438.9932563622</v>
       </c>
       <c r="G19">
-        <f t="shared" si="6"/>
-        <v>65.128148148148</v>
+        <v>4841288.4027576176</v>
       </c>
       <c r="H19">
-        <f t="shared" si="8"/>
-        <v>1533.8278401995378</v>
+        <v>3985902.1319942698</v>
       </c>
       <c r="I19">
-        <f t="shared" si="4"/>
-        <v>-884.05509206134502</v>
+        <v>1115477.2135689086</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
-        <v>1172.9230000000002</v>
+        <v>4842396.1976094702</v>
       </c>
       <c r="K19">
-        <f t="shared" si="5"/>
-        <v>3104.3124354271999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987472.6165894973</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>54</v>
       </c>
@@ -1243,31 +1126,25 @@
         <v>170.142</v>
       </c>
       <c r="F20">
-        <f t="shared" si="7"/>
-        <v>74.123222048432766</v>
+        <v>1116435.3918830184</v>
       </c>
       <c r="G20">
-        <f t="shared" si="6"/>
-        <v>81.640962962962789</v>
+        <v>4841304.9155724328</v>
       </c>
       <c r="H20">
-        <f t="shared" si="8"/>
-        <v>1562.2566824017185</v>
+        <v>3985930.5608364716</v>
       </c>
       <c r="I20">
-        <f t="shared" si="4"/>
-        <v>-839.27402125630533</v>
+        <v>1115521.9946397138</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
-        <v>1124.2714117647063</v>
+        <v>4842347.5460212342</v>
       </c>
       <c r="K20">
-        <f t="shared" si="5"/>
-        <v>3150.581171897622</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987518.8853259678</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>54</v>
       </c>
@@ -1284,31 +1161,25 @@
         <v>171.142</v>
       </c>
       <c r="F21">
-        <f t="shared" si="7"/>
-        <v>70.979037030097388</v>
+        <v>1116432.2476980002</v>
       </c>
       <c r="G21">
-        <f t="shared" si="6"/>
-        <v>98.153777777777577</v>
+        <v>4841321.428387248</v>
       </c>
       <c r="H21">
-        <f t="shared" si="8"/>
-        <v>1588.223183687111</v>
+        <v>3985956.5273377574</v>
       </c>
       <c r="I21">
-        <f t="shared" si="4"/>
-        <v>-793.39025778052155</v>
+        <v>1115567.8784031896</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
-        <v>1075.6198235294121</v>
+        <v>4842298.8944329992</v>
       </c>
       <c r="K21">
-        <f t="shared" si="5"/>
-        <v>3181.7012553260179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987550.0054093963</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>54</v>
       </c>
@@ -1325,31 +1196,25 @@
         <v>172.142</v>
       </c>
       <c r="F22">
-        <f t="shared" si="7"/>
-        <v>68.20301883032343</v>
+        <v>1116429.4716798004</v>
       </c>
       <c r="G22">
-        <f t="shared" si="6"/>
-        <v>114.66659259259239</v>
+        <v>4841337.9412020622</v>
       </c>
       <c r="H22">
-        <f t="shared" si="8"/>
-        <v>1612.120098710149</v>
+        <v>3985980.4242527802</v>
       </c>
       <c r="I22">
-        <f t="shared" si="4"/>
-        <v>-746.37664884143464</v>
+        <v>1115614.8920121286</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
-        <v>1026.9682352941181</v>
+        <v>4842250.2428447641</v>
       </c>
       <c r="K22">
-        <f t="shared" si="5"/>
-        <v>3197.6726857123876</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987565.9768397827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>54</v>
       </c>
@@ -1366,31 +1231,25 @@
         <v>173.142</v>
       </c>
       <c r="F23">
-        <f t="shared" si="7"/>
-        <v>65.728623547772969</v>
+        <v>1116426.9972845179</v>
       </c>
       <c r="G23">
-        <f t="shared" si="6"/>
-        <v>131.17940740740718</v>
+        <v>4841354.4540168773</v>
       </c>
       <c r="H23">
-        <f t="shared" si="8"/>
-        <v>1634.2531141825339</v>
+        <v>3986002.5572682526</v>
       </c>
       <c r="I23">
-        <f t="shared" si="4"/>
-        <v>-698.20537303394985</v>
+        <v>1115663.0632879362</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
-        <v>978.31664705882395</v>
+        <v>4842201.5912565291</v>
       </c>
       <c r="K23">
-        <f t="shared" si="5"/>
-        <v>3198.4954630567308</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987566.799617127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>54</v>
       </c>
@@ -1407,31 +1266,25 @@
         <v>174.142</v>
       </c>
       <c r="F24">
-        <f t="shared" si="7"/>
-        <v>63.504988607630501</v>
+        <v>1116424.7736495777</v>
       </c>
       <c r="G24">
-        <f t="shared" si="6"/>
-        <v>147.692222222222</v>
+        <v>4841370.9668316925</v>
       </c>
       <c r="H24">
-        <f t="shared" si="8"/>
-        <v>1654.8648229757382</v>
+        <v>3986023.1689770459</v>
       </c>
       <c r="I24">
-        <f t="shared" si="4"/>
-        <v>-648.84792387646712</v>
+        <v>1115712.4207370935</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
-        <v>929.66505882352976</v>
+        <v>4842152.9396682931</v>
       </c>
       <c r="K24">
-        <f t="shared" si="5"/>
-        <v>3184.1695873590479</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987552.4737414289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>54</v>
       </c>
@@ -1448,31 +1301,25 @@
         <v>175.142</v>
       </c>
       <c r="F25">
-        <f t="shared" si="7"/>
-        <v>61.492486837908459</v>
+        <v>1116422.7611478081</v>
       </c>
       <c r="G25">
-        <f t="shared" si="6"/>
-        <v>164.20503703703679</v>
+        <v>4841387.4796465067</v>
       </c>
       <c r="H25">
-        <f t="shared" si="8"/>
-        <v>1674.1509754450985</v>
+        <v>3986042.4551295154</v>
       </c>
       <c r="I25">
-        <f t="shared" si="4"/>
-        <v>-598.2750929415015</v>
+        <v>1115762.9935680286</v>
       </c>
       <c r="J25">
-        <f t="shared" si="3"/>
-        <v>881.0134705882358</v>
+        <v>4842104.2880800581</v>
       </c>
       <c r="K25">
-        <f t="shared" si="5"/>
-        <v>3154.6950586193389</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987522.9992126892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>54</v>
       </c>
@@ -1489,31 +1336,25 @@
         <v>176.142</v>
       </c>
       <c r="F26">
-        <f t="shared" si="7"/>
-        <v>59.659728199242565</v>
+        <v>1116420.9283891693</v>
       </c>
       <c r="G26">
-        <f t="shared" si="6"/>
-        <v>180.71785185185161</v>
+        <v>4841403.9924613219</v>
       </c>
       <c r="H26">
-        <f t="shared" si="8"/>
-        <v>1692.2718134191421</v>
+        <v>3986060.5759674893</v>
       </c>
       <c r="I26">
-        <f t="shared" si="4"/>
-        <v>-546.45695257091393</v>
+        <v>1115814.8117083991</v>
       </c>
       <c r="J26">
-        <f t="shared" si="3"/>
-        <v>832.36188235294162</v>
+        <v>4842055.636491823</v>
       </c>
       <c r="K26">
-        <f t="shared" si="5"/>
-        <v>3110.0718768376032</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987478.3760309075</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>54</v>
       </c>
@@ -1530,31 +1371,25 @@
         <v>177.142</v>
       </c>
       <c r="F27">
-        <f t="shared" si="7"/>
-        <v>57.981483771143949</v>
+        <v>1116419.2501447413</v>
       </c>
       <c r="G27">
-        <f t="shared" si="6"/>
-        <v>197.23066666666637</v>
+        <v>4841420.5052761361</v>
       </c>
       <c r="H27">
-        <f t="shared" si="8"/>
-        <v>1709.3601708902436</v>
+        <v>3986077.6643249602</v>
       </c>
       <c r="I27">
-        <f t="shared" si="4"/>
-        <v>-493.36283816551577</v>
+        <v>1115867.9058228044</v>
       </c>
       <c r="J27">
-        <f t="shared" si="3"/>
-        <v>783.71029411764744</v>
+        <v>4842006.984903587</v>
       </c>
       <c r="K27">
-        <f t="shared" si="5"/>
-        <v>3050.3000420138414</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987418.6041960837</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>54</v>
       </c>
@@ -1571,31 +1406,25 @@
         <v>178.142</v>
       </c>
       <c r="F28">
-        <f t="shared" si="7"/>
-        <v>56.437214780531249</v>
+        <v>1116417.7058757506</v>
       </c>
       <c r="G28">
-        <f t="shared" si="6"/>
-        <v>213.74348148148118</v>
+        <v>4841437.0180909513</v>
       </c>
       <c r="H28">
-        <f t="shared" si="8"/>
-        <v>1725.5273887691374</v>
+        <v>3986093.8315428393</v>
       </c>
       <c r="I28">
-        <f t="shared" si="4"/>
-        <v>-438.96133003857449</v>
+        <v>1115922.3073309315</v>
       </c>
       <c r="J28">
-        <f t="shared" si="3"/>
-        <v>735.05870588235348</v>
+        <v>4841958.333315352</v>
       </c>
       <c r="K28">
-        <f t="shared" si="5"/>
-        <v>2975.3795541480536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987343.6837082179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>54</v>
       </c>
@@ -1612,31 +1441,25 @@
         <v>179.142</v>
       </c>
       <c r="F29">
-        <f t="shared" si="7"/>
-        <v>55.010008923110391</v>
+        <v>1116416.278669893</v>
       </c>
       <c r="G29">
-        <f t="shared" si="6"/>
-        <v>230.256296296296</v>
+        <v>4841453.5309057664</v>
       </c>
       <c r="H29">
-        <f t="shared" si="8"/>
-        <v>1740.8677154420159</v>
+        <v>3986109.1718695122</v>
       </c>
       <c r="I29">
-        <f t="shared" si="4"/>
-        <v>-383.22023482247641</v>
+        <v>1115978.0484261476</v>
       </c>
       <c r="J29">
-        <f t="shared" si="3"/>
-        <v>686.40711764705929</v>
+        <v>4841909.6817271169</v>
       </c>
       <c r="K29">
-        <f t="shared" si="5"/>
-        <v>2885.3104132402391</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987253.6145673105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>54</v>
       </c>
@@ -1653,31 +1476,25 @@
         <v>180.142</v>
       </c>
       <c r="F30">
-        <f t="shared" si="7"/>
-        <v>53.685797179294568</v>
+        <v>1116414.9544581494</v>
       </c>
       <c r="G30">
-        <f t="shared" si="6"/>
-        <v>246.76911111111076</v>
+        <v>4841470.0437205806</v>
       </c>
       <c r="H30">
-        <f t="shared" si="8"/>
-        <v>1755.4616357279015</v>
+        <v>3986123.765789798</v>
       </c>
       <c r="I30">
-        <f t="shared" si="4"/>
-        <v>-326.1065664175494</v>
+        <v>1116035.1620945525</v>
       </c>
       <c r="J30">
-        <f t="shared" si="3"/>
-        <v>637.75552941176511</v>
+        <v>4841861.0301388819</v>
       </c>
       <c r="K30">
-        <f t="shared" si="5"/>
-        <v>2780.092619290398</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987148.3967733607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>54</v>
       </c>
@@ -1694,31 +1511,25 @@
         <v>181.142</v>
       </c>
       <c r="F31">
-        <f t="shared" si="7"/>
-        <v>52.452767763044037</v>
+        <v>1116413.7214287331</v>
       </c>
       <c r="G31">
-        <f t="shared" si="6"/>
-        <v>263.28192592592558</v>
+        <v>4841486.5565353958</v>
       </c>
       <c r="H31">
-        <f t="shared" si="8"/>
-        <v>1769.3784268872168</v>
+        <v>3986137.6825809572</v>
       </c>
       <c r="I31">
-        <f t="shared" si="4"/>
-        <v>-267.58652647176268</v>
+        <v>1116093.6821344984</v>
       </c>
       <c r="J31">
-        <f t="shared" si="3"/>
-        <v>589.10394117647115</v>
+        <v>4841812.3785506459</v>
       </c>
       <c r="K31">
-        <f t="shared" si="5"/>
-        <v>2659.7261722985318</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3987028.0303263688</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>54</v>
       </c>
@@ -1735,31 +1546,25 @@
         <v>182.142</v>
       </c>
       <c r="F32">
-        <f t="shared" si="7"/>
-        <v>51.300921161617048</v>
+        <v>1116412.5695821317</v>
       </c>
       <c r="G32">
-        <f t="shared" si="6"/>
-        <v>279.79474074074039</v>
+        <v>4841503.0693502109</v>
       </c>
       <c r="H32">
-        <f t="shared" si="8"/>
-        <v>1782.6781475225544</v>
+        <v>3986150.9823015928</v>
       </c>
       <c r="I32">
-        <f t="shared" si="4"/>
-        <v>-207.62548437976056</v>
+        <v>1116153.6431765903</v>
       </c>
       <c r="J32">
-        <f t="shared" si="3"/>
-        <v>540.45235294117697</v>
+        <v>4841763.7269624108</v>
       </c>
       <c r="K32">
-        <f t="shared" si="5"/>
-        <v>2524.211072264638</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986892.5152263348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>54</v>
       </c>
@@ -1776,31 +1581,25 @@
         <v>183.142</v>
       </c>
       <c r="F33">
-        <f t="shared" si="7"/>
-        <v>50.221727827153508</v>
+        <v>1116411.4903887971</v>
       </c>
       <c r="G33">
-        <f t="shared" si="6"/>
-        <v>296.30755555555515</v>
+        <v>4841519.5821650252</v>
       </c>
       <c r="H33">
-        <f t="shared" si="8"/>
-        <v>1795.4132039685269</v>
+        <v>3986163.7173580388</v>
       </c>
       <c r="I33">
-        <f t="shared" si="4"/>
-        <v>-146.18795678938977</v>
+        <v>1116215.0807041808</v>
       </c>
       <c r="J33">
-        <f t="shared" si="3"/>
-        <v>491.80076470588301</v>
+        <v>4841715.0753741758</v>
       </c>
       <c r="K33">
-        <f t="shared" si="5"/>
-        <v>2373.547319188719</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986741.8514732588</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>54</v>
       </c>
@@ -1817,31 +1616,25 @@
         <v>184.142</v>
       </c>
       <c r="F34">
-        <f t="shared" si="7"/>
-        <v>49.207861672609347</v>
+        <v>1116410.4765226427</v>
       </c>
       <c r="G34">
-        <f t="shared" si="6"/>
-        <v>312.82037037036997</v>
+        <v>4841536.0949798403</v>
       </c>
       <c r="H34">
-        <f t="shared" si="8"/>
-        <v>1807.629597502322</v>
+        <v>3986175.9337515724</v>
       </c>
       <c r="I34">
-        <f t="shared" si="4"/>
-        <v>-83.237586603594991</v>
+        <v>1116278.0310743665</v>
       </c>
       <c r="J34">
-        <f t="shared" ref="J34:J54" si="9">2000-48.6515882352941*(E34-152.142)</f>
-        <v>443.14917647058883</v>
+        <v>4841666.4237859407</v>
       </c>
       <c r="K34">
-        <f t="shared" si="5"/>
-        <v>2207.734913070773</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986576.0390671408</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>54</v>
       </c>
@@ -1858,31 +1651,25 @@
         <v>185.142</v>
       </c>
       <c r="F35">
-        <f t="shared" si="7"/>
-        <v>48.252990309501683</v>
+        <v>1116409.5216512796</v>
       </c>
       <c r="G35">
-        <f t="shared" si="6"/>
-        <v>329.33318518518479</v>
+        <v>4841552.6077946546</v>
       </c>
       <c r="H35">
-        <f t="shared" si="8"/>
-        <v>1819.3679273744299</v>
+        <v>3986187.6720814444</v>
       </c>
       <c r="I35">
-        <f t="shared" si="4"/>
-        <v>-18.737121465253949</v>
+        <v>1116342.5315395049</v>
       </c>
       <c r="J35">
-        <f t="shared" si="9"/>
-        <v>394.49758823529464</v>
+        <v>4841617.7721977048</v>
       </c>
       <c r="K35">
-        <f t="shared" si="5"/>
-        <v>2026.7738539108007</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986395.0780079807</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>54</v>
       </c>
@@ -1899,31 +1686,25 @@
         <v>186.142</v>
       </c>
       <c r="F36">
-        <f t="shared" si="7"/>
-        <v>47.351608287778213</v>
+        <v>1116408.6202692578</v>
       </c>
       <c r="G36">
-        <f t="shared" si="6"/>
-        <v>345.84599999999961</v>
+        <v>4841569.1206094697</v>
       </c>
       <c r="H36">
-        <f t="shared" si="8"/>
-        <v>1830.6642048712795</v>
+        <v>3986198.9683589414</v>
       </c>
       <c r="I36">
-        <f t="shared" si="4"/>
-        <v>47.351608287779072</v>
+        <v>1116408.6202692578</v>
       </c>
       <c r="J36">
-        <f t="shared" si="9"/>
-        <v>345.84600000000069</v>
+        <v>4841569.1206094697</v>
       </c>
       <c r="K36">
-        <f t="shared" si="5"/>
-        <v>1830.6641417088026</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3986198.9682957791</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>54</v>
       </c>
@@ -1940,31 +1721,25 @@
         <v>187.142</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
-        <v>46.498903297628743</v>
+        <v>1116407.7675642676</v>
       </c>
       <c r="G37">
-        <f t="shared" si="6"/>
-        <v>362.35881481481437</v>
+        <v>4841585.6334242849</v>
       </c>
       <c r="H37">
-        <f t="shared" si="8"/>
-        <v>1841.5505195842798</v>
+        <v>3986209.8546736543</v>
       </c>
       <c r="I37">
-        <f t="shared" si="4"/>
-        <v>115.06771221046392</v>
+        <v>1116476.3363731804</v>
       </c>
       <c r="J37">
-        <f t="shared" si="9"/>
-        <v>297.1944117647065</v>
+        <v>4841520.4690212347</v>
       </c>
       <c r="K37">
-        <f t="shared" si="5"/>
-        <v>1619.405776464778</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985987.7099305349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>54</v>
       </c>
@@ -1981,31 +1756,25 @@
         <v>188.142</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
-        <v>45.690647903146484</v>
+        <v>1116406.9593088732</v>
       </c>
       <c r="G38">
-        <f t="shared" si="6"/>
-        <v>378.87162962962918</v>
+        <v>4841602.1462390991</v>
       </c>
       <c r="H38">
-        <f t="shared" si="8"/>
-        <v>1852.0555889587017</v>
+        <v>3986220.3597430289</v>
       </c>
       <c r="I38">
-        <f t="shared" si="4"/>
-        <v>184.45126289457221</v>
+        <v>1116545.7199238646</v>
       </c>
       <c r="J38">
-        <f t="shared" si="9"/>
-        <v>248.54282352941254</v>
+        <v>4841471.8174329996</v>
       </c>
       <c r="K38">
-        <f t="shared" si="5"/>
-        <v>1392.9987581787277</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985761.3029122488</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>54</v>
       </c>
@@ -2022,31 +1791,25 @@
         <v>189.142</v>
       </c>
       <c r="F39">
-        <f t="shared" si="7"/>
-        <v>44.92311124486271</v>
+        <v>1116406.1917722148</v>
       </c>
       <c r="G39">
-        <f t="shared" si="6"/>
-        <v>395.384444444444</v>
+        <v>4841618.6590539142</v>
       </c>
       <c r="H39">
-        <f t="shared" si="8"/>
-        <v>1862.2052148311516</v>
+        <v>3986230.5093689011</v>
       </c>
       <c r="I39">
-        <f t="shared" si="4"/>
-        <v>255.54331968257975</v>
+        <v>1116616.8119806526</v>
       </c>
       <c r="J39">
-        <f t="shared" si="9"/>
-        <v>199.89123529411836</v>
+        <v>4841423.1658447636</v>
       </c>
       <c r="K39">
-        <f t="shared" si="5"/>
-        <v>1151.4430868506497</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985519.7472409206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>54</v>
       </c>
@@ -2063,31 +1826,25 @@
         <v>190.142</v>
       </c>
       <c r="F40">
-        <f t="shared" si="7"/>
-        <v>44.192986500946624</v>
+        <v>1116405.4616474709</v>
       </c>
       <c r="G40">
-        <f t="shared" si="6"/>
-        <v>411.89725925925876</v>
+        <v>4841635.1718687294</v>
       </c>
       <c r="H40">
-        <f t="shared" si="8"/>
-        <v>1872.0226652294282</v>
+        <v>3986240.3268192997</v>
       </c>
       <c r="I40">
-        <f t="shared" si="4"/>
-        <v>328.38595296549965</v>
+        <v>1116689.6546139356</v>
       </c>
       <c r="J40">
-        <f t="shared" si="9"/>
-        <v>151.23964705882418</v>
+        <v>4841374.5142565286</v>
       </c>
       <c r="K40">
-        <f t="shared" si="5"/>
-        <v>894.73876248054614</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3985263.0429165508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -2104,31 +1861,25 @@
         <v>191.142</v>
       </c>
       <c r="F41">
-        <f t="shared" si="7"/>
-        <v>43.497330888627232</v>
+        <v>1116404.7659918587</v>
       </c>
       <c r="G41">
-        <f t="shared" si="6"/>
-        <v>428.41007407407358</v>
+        <v>4841651.6846835436</v>
       </c>
       <c r="H41">
-        <f t="shared" si="8"/>
-        <v>1881.5289956524209</v>
+        <v>3986249.8331497223</v>
       </c>
       <c r="I41">
-        <f t="shared" si="4"/>
-        <v>403.0222690790165</v>
+        <v>1116764.290930049</v>
       </c>
       <c r="J41">
-        <f t="shared" si="9"/>
-        <v>102.58805882353022</v>
+        <v>4841325.8626682935</v>
       </c>
       <c r="K41">
-        <f t="shared" si="5"/>
-        <v>622.88578506841679</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984991.1899391385</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>54</v>
       </c>
@@ -2145,31 +1896,25 @@
         <v>192.142</v>
       </c>
       <c r="F42">
-        <f t="shared" si="7"/>
-        <v>42.83351572252775</v>
+        <v>1116404.1021766926</v>
       </c>
       <c r="G42">
-        <f t="shared" si="6"/>
-        <v>444.92288888888834</v>
+        <v>4841668.1974983588</v>
       </c>
       <c r="H42">
-        <f t="shared" si="8"/>
-        <v>1890.7433209889703</v>
+        <v>3986259.0474750591</v>
       </c>
       <c r="I42">
-        <f t="shared" si="4"/>
-        <v>479.49643581267856</v>
+        <v>1116840.7650967827</v>
       </c>
       <c r="J42">
-        <f t="shared" si="9"/>
-        <v>53.936470588236034</v>
+        <v>4841277.2110800585</v>
       </c>
       <c r="K42">
-        <f t="shared" si="5"/>
-        <v>335.8841546142603</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984704.1883086842</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>54</v>
       </c>
@@ -2186,31 +1931,25 @@
         <v>193.142</v>
       </c>
       <c r="F43">
-        <f t="shared" si="7"/>
-        <v>42.199184597099901</v>
+        <v>1116403.467845567</v>
       </c>
       <c r="G43">
-        <f t="shared" si="6"/>
-        <v>461.43570370370321</v>
+        <v>4841684.7103131739</v>
       </c>
       <c r="H43">
-        <f t="shared" si="8"/>
-        <v>1899.6830469055694</v>
+        <v>3986267.9872009759</v>
       </c>
       <c r="I43">
-        <f t="shared" si="4"/>
-        <v>557.85370854721305</v>
+        <v>1116919.1223695173</v>
       </c>
       <c r="J43">
-        <f t="shared" si="9"/>
-        <v>5.2848823529418496</v>
+        <v>4841228.5594918225</v>
       </c>
       <c r="K43">
-        <f t="shared" si="5"/>
-        <v>33.73387111807773</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984402.0380251883</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>54</v>
       </c>
@@ -2227,31 +1966,25 @@
         <v>194.142</v>
       </c>
       <c r="F44">
-        <f t="shared" si="7"/>
-        <v>41.592218176547647</v>
+        <v>1116402.8608791465</v>
       </c>
       <c r="G44">
-        <f t="shared" si="6"/>
-        <v>477.94851851851797</v>
+        <v>4841701.2231279882</v>
       </c>
       <c r="H44">
-        <f t="shared" si="8"/>
-        <v>1908.3640677432238</v>
+        <v>3986276.6682218132</v>
       </c>
       <c r="I44">
-        <f t="shared" si="4"/>
-        <v>638.14045703546572</v>
+        <v>1116999.4091180055</v>
       </c>
       <c r="J44">
-        <f t="shared" si="9"/>
-        <v>-43.366705882352107</v>
+        <v>4841179.9079035874</v>
       </c>
       <c r="K44">
-        <f t="shared" si="5"/>
-        <v>-283.56506542013022</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3984084.7390886499</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>54</v>
       </c>
@@ -2268,31 +2001,25 @@
         <v>195.142</v>
       </c>
       <c r="F45">
-        <f t="shared" si="7"/>
-        <v>41.010704393115105</v>
+        <v>1116402.2793653631</v>
       </c>
       <c r="G45">
-        <f t="shared" si="6"/>
-        <v>494.46133333333273</v>
+        <v>4841717.7359428033</v>
       </c>
       <c r="H45">
-        <f t="shared" si="8"/>
-        <v>1916.8009365771138</v>
+        <v>3986285.105090647</v>
       </c>
       <c r="I45">
-        <f t="shared" si="4"/>
-        <v>720.40419284278778</v>
+        <v>1117081.6728538128</v>
       </c>
       <c r="J45">
-        <f t="shared" si="9"/>
-        <v>-92.018294117646292</v>
+        <v>4841131.2563153524</v>
       </c>
       <c r="K45">
-        <f t="shared" si="5"/>
-        <v>-616.01265500036538</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3983752.2914990699</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>54</v>
       </c>
@@ -2309,31 +2036,25 @@
         <v>196.142</v>
       </c>
       <c r="F46">
-        <f t="shared" si="7"/>
-        <v>40.452913098834031</v>
+        <v>1116401.7215740688</v>
       </c>
       <c r="G46">
-        <f t="shared" si="6"/>
-        <v>510.97414814814761</v>
+        <v>4841734.2487576175</v>
       </c>
       <c r="H46">
-        <f t="shared" si="8"/>
-        <v>1925.0070120096393</v>
+        <v>3986293.3111660797</v>
       </c>
       <c r="I46">
-        <f t="shared" si="4"/>
-        <v>804.69359746311648</v>
+        <v>1117165.9622584332</v>
       </c>
       <c r="J46">
-        <f t="shared" si="9"/>
-        <v>-140.66988235294048</v>
+        <v>4841082.6047271164</v>
       </c>
       <c r="K46">
-        <f t="shared" si="5"/>
-        <v>-963.60889762262764</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3983404.6952564474</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>54</v>
       </c>
@@ -2350,31 +2071,25 @@
         <v>197.142</v>
       </c>
       <c r="F47">
-        <f t="shared" si="7"/>
-        <v>39.917274405182958</v>
+        <v>1116401.1859353753</v>
       </c>
       <c r="G47">
-        <f t="shared" si="6"/>
-        <v>527.48696296296237</v>
+        <v>4841750.7615724327</v>
       </c>
       <c r="H47">
-        <f t="shared" si="8"/>
-        <v>1932.9945854151747</v>
+        <v>3986301.2987394854</v>
       </c>
       <c r="I47">
-        <f t="shared" si="4"/>
-        <v>891.05855112739027</v>
+        <v>1117252.3272120974</v>
       </c>
       <c r="J47">
-        <f t="shared" si="9"/>
-        <v>-189.32147058823466</v>
+        <v>4841033.9531388814</v>
       </c>
       <c r="K47">
-        <f t="shared" si="5"/>
-        <v>-1326.3537932869156</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3983041.9503607834</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>54</v>
       </c>
@@ -2391,31 +2106,25 @@
         <v>198.142</v>
       </c>
       <c r="F48">
-        <f t="shared" si="7"/>
-        <v>39.402360093009371</v>
+        <v>1116400.6710210631</v>
       </c>
       <c r="G48">
-        <f t="shared" si="6"/>
-        <v>543.99977777777713</v>
+        <v>4841767.2743872479</v>
       </c>
       <c r="H48">
-        <f t="shared" si="8"/>
-        <v>1940.7749916795403</v>
+        <v>3986309.0791457496</v>
       </c>
       <c r="I48">
-        <f t="shared" si="4"/>
-        <v>979.55016232134585</v>
+        <v>1117340.8188232915</v>
       </c>
       <c r="J48">
-        <f t="shared" si="9"/>
-        <v>-237.97305882352839</v>
+        <v>4840985.3015506463</v>
       </c>
       <c r="K48">
-        <f t="shared" si="5"/>
-        <v>-1704.2473419932271</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3982664.0568120768</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>54</v>
       </c>
@@ -2432,31 +2141,25 @@
         <v>199.142</v>
       </c>
       <c r="F49">
-        <f t="shared" si="7"/>
-        <v>38.906867591406339</v>
+        <v>1116400.1755285615</v>
       </c>
       <c r="G49">
-        <f t="shared" si="6"/>
-        <v>560.512592592592</v>
+        <v>4841783.7872020621</v>
       </c>
       <c r="H49">
-        <f t="shared" si="8"/>
-        <v>1948.3587059384915</v>
+        <v>3986316.6628600084</v>
       </c>
       <c r="I49">
-        <f t="shared" si="4"/>
-        <v>1070.2207980301641</v>
+        <v>1117431.4894590003</v>
       </c>
       <c r="J49">
-        <f t="shared" si="9"/>
-        <v>-286.62464705882257</v>
+        <v>4840936.6499624113</v>
       </c>
       <c r="K49">
-        <f t="shared" si="5"/>
-        <v>-2097.2895437415673</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3982271.0146103287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>54</v>
       </c>
@@ -2473,31 +2176,25 @@
         <v>200.142</v>
       </c>
       <c r="F50">
-        <f t="shared" si="7"/>
-        <v>38.429606116348921</v>
+        <v>1116399.6982670864</v>
       </c>
       <c r="G50">
-        <f t="shared" si="6"/>
-        <v>577.02540740740676</v>
+        <v>4841800.3000168772</v>
       </c>
       <c r="H50">
-        <f t="shared" si="8"/>
-        <v>1955.755428387145</v>
+        <v>3986324.0595824574</v>
       </c>
       <c r="I50">
-        <f t="shared" si="4"/>
-        <v>1163.1241147278561</v>
+        <v>1117524.3927756979</v>
       </c>
       <c r="J50">
-        <f t="shared" si="9"/>
-        <v>-335.27623529411676</v>
+        <v>4840887.9983741753</v>
       </c>
       <c r="K50">
-        <f t="shared" si="5"/>
-        <v>-2505.4803985319345</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3981862.8237555381</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>54</v>
       </c>
@@ -2514,31 +2211,25 @@
         <v>201.142</v>
       </c>
       <c r="F51">
-        <f t="shared" si="7"/>
-        <v>37.969484633290413</v>
+        <v>1116399.2381456033</v>
       </c>
       <c r="G51">
-        <f t="shared" si="6"/>
-        <v>593.53822222222152</v>
+        <v>4841816.8128316924</v>
       </c>
       <c r="H51">
-        <f t="shared" si="8"/>
-        <v>1962.9741588831439</v>
+        <v>3986331.2783129532</v>
       </c>
       <c r="I51">
-        <f t="shared" si="4"/>
-        <v>1258.3150901297445</v>
+        <v>1117619.5837510999</v>
       </c>
       <c r="J51">
-        <f t="shared" si="9"/>
-        <v>-383.92782352941094</v>
+        <v>4840839.3467859402</v>
       </c>
       <c r="K51">
-        <f t="shared" si="5"/>
-        <v>-2928.8199063643278</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3981439.4842477059</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>54</v>
       </c>
@@ -2555,31 +2246,25 @@
         <v>202.142</v>
       </c>
       <c r="F52">
-        <f t="shared" si="7"/>
-        <v>37.525501366746298</v>
+        <v>1116398.7941623367</v>
       </c>
       <c r="G52">
-        <f t="shared" si="6"/>
-        <v>610.05103703703639</v>
+        <v>4841833.3256465066</v>
       </c>
       <c r="H52">
-        <f t="shared" si="8"/>
-        <v>1970.0232627828932</v>
+        <v>3986338.327416853</v>
       </c>
       <c r="I52">
-        <f t="shared" si="4"/>
-        <v>1355.8500557268139</v>
+        <v>1117717.1187166967</v>
       </c>
       <c r="J52">
-        <f t="shared" si="9"/>
-        <v>-432.57941176470513</v>
+        <v>4840790.6951977052</v>
       </c>
       <c r="K52">
-        <f t="shared" si="5"/>
-        <v>-3367.3080672387468</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3981000.9960868312</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>54</v>
       </c>
@@ -2596,31 +2281,25 @@
         <v>203.142</v>
       </c>
       <c r="F53">
-        <f t="shared" si="7"/>
-        <v>37.096734627304933</v>
+        <v>1116398.3653955974</v>
       </c>
       <c r="G53">
-        <f t="shared" si="6"/>
-        <v>626.56385185185115</v>
+        <v>4841849.8384613218</v>
       </c>
       <c r="H53">
-        <f t="shared" si="8"/>
-        <v>1976.9105292188128</v>
+        <v>3986345.2146832887</v>
       </c>
       <c r="I53">
-        <f t="shared" si="4"/>
-        <v>1455.7867301211859</v>
+        <v>1117817.0553910912</v>
       </c>
       <c r="J53">
-        <f t="shared" si="9"/>
-        <v>-481.23099999999886</v>
+        <v>4840742.0436094701</v>
       </c>
       <c r="K53">
-        <f t="shared" si="5"/>
-        <v>-3820.9448811551893</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+        <v>3980547.3592729149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2637,33 +2316,28 @@
         <v>204.142</v>
       </c>
       <c r="F54">
-        <f t="shared" si="7"/>
-        <v>36.68233476492955</v>
+        <v>1116397.9509957349</v>
       </c>
       <c r="G54">
-        <f t="shared" si="6"/>
-        <v>643.07666666666591</v>
+        <v>4841866.3512761369</v>
       </c>
       <c r="H54">
-        <f t="shared" si="8"/>
-        <v>1983.6432228357412</v>
+        <v>3986351.9473769059</v>
       </c>
       <c r="I54">
-        <f t="shared" si="4"/>
-        <v>1558.1842531824664</v>
+        <v>1117919.4529141525</v>
       </c>
       <c r="J54">
-        <f t="shared" si="9"/>
-        <v>-529.88258823529304</v>
+        <v>4840693.3920212341</v>
       </c>
       <c r="K54">
-        <f t="shared" si="5"/>
-        <v>-4289.7303481136614</v>
+        <v>3980078.5738059566</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2826,18 +2500,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2859,25 +2533,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF81D76D-6B47-4763-B248-A734C6973102}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{598D0E15-7304-4366-8C1A-B5658ED50470}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a57214d9-3dcc-43e0-a8c0-da7fb2d093ec"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{598D0E15-7304-4366-8C1A-B5658ED50470}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF81D76D-6B47-4763-B248-A734C6973102}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a57214d9-3dcc-43e0-a8c0-da7fb2d093ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>